<commit_message>
Ultimos updates y mouse erratico
</commit_message>
<xml_diff>
--- a/citas/CARTAGO_citas_disponibles.xlsx
+++ b/citas/CARTAGO_citas_disponibles.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jueves 16/05/2024</t>
+          <t>Martes 14/05/2024</t>
         </is>
       </c>
     </row>
@@ -453,7 +453,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Viernes 17/05/2024</t>
+          <t>Miércoles 15/05/2024</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jueves 23/05/2024</t>
+          <t>Lunes 27/05/2024</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Lunes 27/05/2024</t>
+          <t>Martes 28/05/2024</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Martes 28/05/2024</t>
+          <t>Miércoles 29/05/2024</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Miércoles 29/05/2024</t>
+          <t>Lunes 03/06/2024</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Jueves 30/05/2024</t>
+          <t>Martes 04/06/2024</t>
         </is>
       </c>
     </row>

</xml_diff>